<commit_message>
BG task of day.
</commit_message>
<xml_diff>
--- a/Gimmix/FE.xlsx
+++ b/Gimmix/FE.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
   <si>
     <t>Class</t>
   </si>
@@ -282,21 +282,9 @@
     <t>Dark Lance</t>
   </si>
   <si>
-    <t>Gun Lance</t>
-  </si>
-  <si>
-    <t>Bow Lance</t>
-  </si>
-  <si>
     <t>Light Anima</t>
   </si>
   <si>
-    <t>Dark Gun</t>
-  </si>
-  <si>
-    <t>Light Shield</t>
-  </si>
-  <si>
     <t>Light Bow</t>
   </si>
   <si>
@@ -318,15 +306,9 @@
     <t>Crossbowman</t>
   </si>
   <si>
-    <t>DemonSlayer</t>
-  </si>
-  <si>
     <t>DragonKnight</t>
   </si>
   <si>
-    <t>Exorcist</t>
-  </si>
-  <si>
     <t>Flamecaller</t>
   </si>
   <si>
@@ -345,18 +327,9 @@
     <t>Mercedes</t>
   </si>
   <si>
-    <t>Myrmidon</t>
-  </si>
-  <si>
     <t>PortalMage</t>
   </si>
   <si>
-    <t>Rioter</t>
-  </si>
-  <si>
-    <t>WildHunter</t>
-  </si>
-  <si>
     <t>Berserker</t>
   </si>
   <si>
@@ -364,6 +337,42 @@
   </si>
   <si>
     <t>ReflectorMage</t>
+  </si>
+  <si>
+    <t>Cannon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = </t>
+  </si>
+  <si>
+    <t>GunLance</t>
+  </si>
+  <si>
+    <t>MarauderGer</t>
+  </si>
+  <si>
+    <t>SoulSpear</t>
+  </si>
+  <si>
+    <t>Holy Arrow</t>
+  </si>
+  <si>
+    <t>Regenerate</t>
+  </si>
+  <si>
+    <t>Flame Wizard</t>
+  </si>
+  <si>
+    <t>Blue Mage</t>
+  </si>
+  <si>
+    <t>Wind Breaker</t>
+  </si>
+  <si>
+    <t>Lieutenants</t>
+  </si>
+  <si>
+    <t>Monk</t>
   </si>
 </sst>
 </file>
@@ -477,47 +486,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1609,25 +1578,25 @@
     <sortCondition descending="1" ref="D2:D30"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1642,7 +1611,7 @@
   <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1673,7 +1642,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="3">
-        <f>SUM(G2:G31)</f>
+        <f>SUM(G2:G32)</f>
         <v>100</v>
       </c>
     </row>
@@ -1682,229 +1651,229 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D2" s="1">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="E2">
         <f>SUM((100*D2)/2048)</f>
-        <v>7.03125</v>
+        <v>8.935546875</v>
       </c>
       <c r="G2">
-        <f>SUM(E2:E4)</f>
-        <v>19.189453125</v>
+        <f>SUM(E2:E6)</f>
+        <v>33.49609375</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E3">
         <f>SUM((100*D3)/2048)</f>
-        <v>6.15234375</v>
+        <v>6.640625</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E4">
         <f>SUM((100*D4)/2048)</f>
-        <v>6.005859375</v>
+        <v>6.103515625</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E5">
         <f>SUM((100*D5)/2048)</f>
-        <v>5.712890625</v>
-      </c>
-      <c r="G5">
-        <f>SUM(E5:E30)</f>
-        <v>75.048828125</v>
+        <v>5.95703125</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E6">
         <f>SUM((100*D6)/2048)</f>
-        <v>4.39453125</v>
+        <v>5.859375</v>
       </c>
     </row>
     <row r="7" spans="2:7">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E7">
         <f>SUM((100*D7)/2048)</f>
-        <v>4.345703125</v>
+        <v>4.19921875</v>
+      </c>
+      <c r="G7">
+        <f>SUM(E7:E31)</f>
+        <v>62.01171875</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E8">
         <f>SUM((100*D8)/2048)</f>
-        <v>4.296875</v>
+        <v>4.1015625</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E9">
         <f>SUM((100*D9)/2048)</f>
-        <v>3.7109375</v>
+        <v>3.857421875</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E10">
         <f>SUM((100*D10)/2048)</f>
-        <v>3.7109375</v>
+        <v>3.80859375</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="D11" s="1">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11">
         <f>SUM((100*D11)/2048)</f>
-        <v>3.7109375</v>
+        <v>3.61328125</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E12">
         <f>SUM((100*D12)/2048)</f>
-        <v>3.3203125</v>
+        <v>3.564453125</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E13">
         <f>SUM((100*D13)/2048)</f>
-        <v>3.3203125</v>
+        <v>3.41796875</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D14" s="1">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E14">
         <f>SUM((100*D14)/2048)</f>
-        <v>3.02734375</v>
+        <v>3.173828125</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15">
         <f>SUM((100*D15)/2048)</f>
-        <v>2.978515625</v>
+        <v>3.02734375</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E16">
         <f>SUM((100*D16)/2048)</f>
-        <v>2.83203125</v>
+        <v>2.685546875</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E17">
         <f>SUM((100*D17)/2048)</f>
-        <v>2.685546875</v>
+        <v>2.490234375</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E18">
         <f>SUM((100*D18)/2048)</f>
-        <v>2.587890625</v>
+        <v>2.44140625</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D19" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E19">
         <f>SUM((100*D19)/2048)</f>
-        <v>2.587890625</v>
+        <v>2.34375</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>15</v>
@@ -1916,194 +1885,194 @@
     </row>
     <row r="20" spans="2:10">
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D20" s="1">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E20">
         <f>SUM((100*D20)/2048)</f>
-        <v>2.34375</v>
+        <v>2.05078125</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <f>SUM((100*D21)/2048)</f>
-        <v>2.24609375</v>
+        <v>2.001953125</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D22" s="1">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E22">
         <f>SUM((100*D22)/2048)</f>
-        <v>2.24609375</v>
+        <v>1.806640625</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E23">
         <f>SUM((100*D23)/2048)</f>
-        <v>2.24609375</v>
+        <v>1.806640625</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="C24" s="1" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <f>SUM((100*D24)/2048)</f>
-        <v>2.099609375</v>
+        <v>1.7578125</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E25">
         <f>SUM((100*D25)/2048)</f>
-        <v>2.05078125</v>
+        <v>1.66015625</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="C26" s="1" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="D26" s="1">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E26">
         <f>SUM((100*D26)/2048)</f>
-        <v>1.85546875</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="C27" s="1" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D27" s="1">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E27">
         <f>SUM((100*D27)/2048)</f>
-        <v>1.85546875</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="C28" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D28" s="1">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E28">
         <f>SUM((100*D28)/2048)</f>
-        <v>1.806640625</v>
+        <v>1.46484375</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="C29" s="1" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E29">
         <f>SUM((100*D29)/2048)</f>
-        <v>1.5625</v>
+        <v>1.26953125</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E30">
         <f>SUM((100*D30)/2048)</f>
-        <v>1.513671875</v>
+        <v>1.171875</v>
       </c>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="D31" s="1">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E31">
         <f>SUM((100*D31)/2048)</f>
-        <v>1.513671875</v>
-      </c>
-      <c r="G31">
-        <f>SUM(E31:E39)</f>
-        <v>5.76171875</v>
+        <v>1.171875</v>
       </c>
     </row>
     <row r="32" spans="2:10">
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E32">
         <f>SUM((100*D32)/2048)</f>
-        <v>1.46484375</v>
+        <v>0.9765625</v>
+      </c>
+      <c r="G32">
+        <f>SUM(E32:E39)</f>
+        <v>4.4921875</v>
       </c>
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E33">
         <f>SUM((100*D33)/2048)</f>
-        <v>1.416015625</v>
+        <v>0.927734375</v>
       </c>
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E34">
         <f>SUM((100*D34)/2048)</f>
-        <v>0.537109375</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1">
         <v>11</v>
@@ -2115,50 +2084,44 @@
     </row>
     <row r="36" spans="3:6">
       <c r="C36" s="1" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="D36" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E36">
         <f>SUM((100*D36)/2048)</f>
-        <v>0.146484375</v>
+        <v>0.48828125</v>
       </c>
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="1" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E37">
         <f>SUM((100*D37)/2048)</f>
-        <v>4.8828125E-2</v>
+        <v>0.439453125</v>
       </c>
     </row>
     <row r="38" spans="3:6">
       <c r="C38" s="1" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <f>SUM((100*D38)/2048)</f>
-        <v>4.8828125E-2</v>
+        <v>0.341796875</v>
       </c>
     </row>
     <row r="39" spans="3:6">
-      <c r="C39" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
       <c r="E39">
         <f>SUM((100*D39)/2048)</f>
-        <v>4.8828125E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="3:6">
@@ -2171,39 +2134,39 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="C2:E39">
-    <sortCondition descending="1" ref="D2:D39"/>
+  <sortState ref="C2:E38">
+    <sortCondition descending="1" ref="D2:D38"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E39">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2214,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2416,38 +2379,69 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="1" t="s">
+    <row r="15" spans="1:11">
+      <c r="D15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="16" spans="1:11">
+      <c r="D16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="1" t="s">
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="1" t="s">
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="1" t="s">
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="C14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3125,25 +3119,25 @@
     <sortCondition descending="1" ref="D3:D30"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
RU draft setup. Trading implemented.
</commit_message>
<xml_diff>
--- a/Gimmix/FE.xlsx
+++ b/Gimmix/FE.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
   <si>
     <t>Class</t>
   </si>
@@ -306,12 +306,6 @@
     <t>Crossbowman</t>
   </si>
   <si>
-    <t>DragonKnight</t>
-  </si>
-  <si>
-    <t>Flamecaller</t>
-  </si>
-  <si>
     <t>Gunmaster</t>
   </si>
   <si>
@@ -363,16 +357,19 @@
     <t>Flame Wizard</t>
   </si>
   <si>
-    <t>Blue Mage</t>
-  </si>
-  <si>
-    <t>Wind Breaker</t>
-  </si>
-  <si>
-    <t>Lieutenants</t>
-  </si>
-  <si>
     <t>Monk</t>
+  </si>
+  <si>
+    <t>Dragon Knight</t>
+  </si>
+  <si>
+    <t>Shiva</t>
+  </si>
+  <si>
+    <t>Jett</t>
+  </si>
+  <si>
+    <t>Beginner</t>
   </si>
 </sst>
 </file>
@@ -1610,8 +1607,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1643,7 +1640,7 @@
       </c>
       <c r="G1" s="3">
         <f>SUM(G2:G32)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:7">
@@ -1651,66 +1648,51 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="1">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="E2">
         <f>SUM((100*D2)/2048)</f>
-        <v>8.935546875</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>SUM(E2:E6)</f>
-        <v>33.49609375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1">
-        <v>136</v>
-      </c>
       <c r="E3">
         <f>SUM((100*D3)/2048)</f>
-        <v>6.640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="E4">
         <f>SUM((100*D4)/2048)</f>
-        <v>6.103515625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="1">
-        <v>122</v>
-      </c>
       <c r="E5">
         <f>SUM((100*D5)/2048)</f>
-        <v>5.95703125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="E6">
         <f>SUM((100*D6)/2048)</f>
-        <v>5.859375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -1718,313 +1700,238 @@
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="1">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <f>SUM((100*D7)/2048)</f>
-        <v>4.19921875</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f>SUM(E7:E31)</f>
-        <v>62.01171875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="C8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="1">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <f>SUM((100*D8)/2048)</f>
-        <v>4.1015625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="1">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E9">
         <f>SUM((100*D9)/2048)</f>
-        <v>3.857421875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="C10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E10">
         <f>SUM((100*D10)/2048)</f>
-        <v>3.80859375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="C11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="1">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E11">
         <f>SUM((100*D11)/2048)</f>
-        <v>3.61328125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="C12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="1">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="E12">
         <f>SUM((100*D12)/2048)</f>
-        <v>3.564453125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="E13">
         <f>SUM((100*D13)/2048)</f>
-        <v>3.41796875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="C14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="1">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E14">
         <f>SUM((100*D14)/2048)</f>
-        <v>3.173828125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E15">
         <f>SUM((100*D15)/2048)</f>
-        <v>3.02734375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="1">
-        <v>55</v>
-      </c>
       <c r="E16">
         <f>SUM((100*D16)/2048)</f>
-        <v>2.685546875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="C17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="1">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E17">
         <f>SUM((100*D17)/2048)</f>
-        <v>2.490234375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="C18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="1">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="E18">
         <f>SUM((100*D18)/2048)</f>
-        <v>2.44140625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="C19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="1">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="E19">
         <f>SUM((100*D19)/2048)</f>
-        <v>2.34375</v>
+        <v>0</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="3">
         <f>SUM(G2:G33)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="C20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="1">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <f>SUM((100*D20)/2048)</f>
-        <v>2.05078125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="C21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="1">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E21">
         <f>SUM((100*D21)/2048)</f>
-        <v>2.001953125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="C22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="1">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E22">
         <f>SUM((100*D22)/2048)</f>
-        <v>1.806640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="C23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="1">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="E23">
         <f>SUM((100*D23)/2048)</f>
-        <v>1.806640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="1">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E24">
         <f>SUM((100*D24)/2048)</f>
-        <v>1.7578125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E25">
         <f>SUM((100*D25)/2048)</f>
-        <v>1.66015625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="1">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="E26">
         <f>SUM((100*D26)/2048)</f>
-        <v>1.5625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="C27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="1">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="E27">
         <f>SUM((100*D27)/2048)</f>
-        <v>1.5625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="C28" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E28">
         <f>SUM((100*D28)/2048)</f>
-        <v>1.46484375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="C29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E29">
         <f>SUM((100*D29)/2048)</f>
-        <v>1.26953125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="E30">
         <f>SUM((100*D30)/2048)</f>
-        <v>1.171875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="C31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="1">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E31">
         <f>SUM((100*D31)/2048)</f>
-        <v>1.171875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -2032,90 +1939,63 @@
         <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="1">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E32">
         <f>SUM((100*D32)/2048)</f>
-        <v>0.9765625</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <f>SUM(E32:E39)</f>
-        <v>4.4921875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="1">
-        <v>19</v>
-      </c>
       <c r="E33">
         <f>SUM((100*D33)/2048)</f>
-        <v>0.927734375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="1">
-        <v>16</v>
-      </c>
       <c r="E34">
         <f>SUM((100*D34)/2048)</f>
-        <v>0.78125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35" s="1">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E35">
         <f>SUM((100*D35)/2048)</f>
-        <v>0.537109375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="3:6">
       <c r="C36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="1">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="E36">
         <f>SUM((100*D36)/2048)</f>
-        <v>0.48828125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:6">
-      <c r="C37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="1">
-        <v>9</v>
-      </c>
       <c r="E37">
         <f>SUM((100*D37)/2048)</f>
-        <v>0.439453125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="3:6">
-      <c r="C38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="1">
-        <v>7</v>
-      </c>
       <c r="E38">
         <f>SUM((100*D38)/2048)</f>
-        <v>0.341796875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="3:6">
@@ -2130,12 +2010,12 @@
       </c>
       <c r="F40" s="3">
         <f>SUM(G2:G39)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="C2:E38">
-    <sortCondition descending="1" ref="D2:D38"/>
+  <sortState ref="C2:E39">
+    <sortCondition descending="1" ref="D2:D39"/>
   </sortState>
   <conditionalFormatting sqref="C16:C24">
     <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
@@ -2391,21 +2271,21 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>81</v>
@@ -2413,10 +2293,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>82</v>
@@ -2424,10 +2304,10 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>84</v>
@@ -2435,10 +2315,10 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>83</v>

</xml_diff>